<commit_message>
L171-L176: Tuning/bug fixes & enemy rebulds (partial)
</commit_message>
<xml_diff>
--- a/Assets/RPG Stats Spreadsheet.xlsx
+++ b/Assets/RPG Stats Spreadsheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="576" windowWidth="22716" windowHeight="11052" activeTab="4"/>
+    <workbookView xWindow="132" yWindow="576" windowWidth="22716" windowHeight="11052" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Soul" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="131">
   <si>
     <t>Player Details</t>
   </si>
@@ -558,15 +558,6 @@
     <t>Unarmed Cast D A1 - A3</t>
   </si>
   <si>
-    <t>2 Hand Sword A1</t>
-  </si>
-  <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>2 Hand Sword A10</t>
-  </si>
-  <si>
     <t>Unarmed Block</t>
   </si>
   <si>
@@ -634,6 +625,9 @@
   </si>
   <si>
     <t>Trigger Radius</t>
+  </si>
+  <si>
+    <t>2 Hand Sword A1 - A10</t>
   </si>
 </sst>
 </file>
@@ -751,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -842,6 +836,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1069,11 +1066,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="92080000"/>
-        <c:axId val="92081536"/>
+        <c:axId val="91490176"/>
+        <c:axId val="91491712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="92080000"/>
+        <c:axId val="91490176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,13 +1087,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92081536"/>
+        <c:crossAx val="91491712"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="92081536"/>
+        <c:axId val="91491712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1115,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="92080000"/>
+        <c:crossAx val="91490176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1129,10 +1126,12 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.85156358281909028"/>
-          <c:y val="0.48913134338893827"/>
-          <c:w val="0.13411475386906163"/>
-          <c:h val="0.12826110782198824"/>
+          <c:wMode val="edge"/>
+          <c:hMode val="edge"/>
+          <c:x val="0.85156352526246715"/>
+          <c:y val="0.48913129065388561"/>
+          <c:w val="0.98567827947287834"/>
+          <c:h val="0.61739244550952865"/>
         </c:manualLayout>
       </c:layout>
     </c:legend>
@@ -1140,7 +1139,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -30523,8 +30522,8 @@
   </sheetPr>
   <dimension ref="A1:AB1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -69702,7 +69701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B16" sqref="B16"/>
       <selection pane="topRight" activeCell="B16" sqref="B16"/>
@@ -69939,10 +69938,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -70131,43 +70130,31 @@
       <c r="A26" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>107</v>
+      <c r="B26" s="45" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="34"/>
-      <c r="B27" s="34" t="s">
-        <v>108</v>
-      </c>
+      <c r="B27" s="34"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="34"/>
+      <c r="A28" s="34" t="s">
+        <v>71</v>
+      </c>
       <c r="B28" s="34" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="34"/>
-      <c r="B29" s="34"/>
+      <c r="B29" s="34" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="34" t="s">
-        <v>71</v>
-      </c>
-      <c r="B30" s="34" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="34"/>
-      <c r="B31" s="34" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" s="34"/>
-      <c r="B32" s="34"/>
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
     </row>
   </sheetData>
   <phoneticPr fontId="10" type="noConversion"/>
@@ -70198,12 +70185,12 @@
   <sheetData>
     <row r="1" spans="1:22" ht="21">
       <c r="A1" s="31" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="33" customFormat="1">
       <c r="A3" s="33" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B3" s="33">
         <v>1</v>
@@ -70271,7 +70258,7 @@
     </row>
     <row r="4" spans="1:22" s="34" customFormat="1">
       <c r="A4" s="34" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B4" s="34">
         <v>1</v>
@@ -70279,7 +70266,7 @@
     </row>
     <row r="5" spans="1:22" s="34" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B5" s="34">
         <v>1.5</v>
@@ -70287,7 +70274,7 @@
     </row>
     <row r="6" spans="1:22" s="44" customFormat="1">
       <c r="A6" s="36" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B6" s="44" t="s">
         <v>80</v>
@@ -70295,7 +70282,7 @@
     </row>
     <row r="7" spans="1:22" s="34" customFormat="1">
       <c r="A7" s="34" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>70</v>
@@ -70314,7 +70301,7 @@
     <row r="10" spans="1:22" s="34" customFormat="1"/>
     <row r="11" spans="1:22" s="34" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B11" s="34">
         <v>5</v>
@@ -70336,15 +70323,15 @@
       <selection activeCell="B4" sqref="B4"/>
       <selection pane="topRight" activeCell="B4" sqref="B4"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22:IV22"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1:D65536"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="19.44140625" style="32" customWidth="1"/>
-    <col min="2" max="4" width="8.88671875" style="32"/>
-    <col min="5" max="5" width="9.109375" style="32" customWidth="1"/>
-    <col min="6" max="9" width="8.88671875" style="32"/>
+    <col min="2" max="2" width="8.88671875" style="32"/>
+    <col min="3" max="3" width="9.109375" style="32" customWidth="1"/>
+    <col min="4" max="9" width="8.88671875" style="32"/>
     <col min="10" max="10" width="9.5546875" style="32" customWidth="1"/>
     <col min="11" max="11" width="11.109375" style="32" customWidth="1"/>
     <col min="12" max="16384" width="8.88671875" style="32"/>
@@ -70352,7 +70339,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21">
       <c r="A1" s="31" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="37" customFormat="1" ht="26.4">
@@ -70360,65 +70347,65 @@
         <v>25</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>26</v>
+        <v>117</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="37" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="G3" s="37" t="s">
         <v>32</v>
       </c>
       <c r="I3" s="37" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="34" customFormat="1">
       <c r="A4" s="34" t="s">
-        <v>124</v>
-      </c>
-      <c r="F4" s="34">
+        <v>121</v>
+      </c>
+      <c r="B4" s="34">
         <v>0.7</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="34" customFormat="1">
       <c r="A5" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="F5" s="34">
+        <v>112</v>
+      </c>
+      <c r="B5" s="34">
         <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="34" customFormat="1"/>
     <row r="7" spans="1:11" s="34" customFormat="1">
       <c r="A7" s="44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C7" s="34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>80</v>
       </c>
+      <c r="E7" s="34" t="s">
+        <v>81</v>
+      </c>
       <c r="F7" s="34" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I7" s="34" t="s">
         <v>80</v>
@@ -70441,33 +70428,33 @@
     </row>
     <row r="10" spans="1:11" s="34" customFormat="1">
       <c r="A10" s="44" t="s">
-        <v>126</v>
-      </c>
-      <c r="F10" s="34">
+        <v>123</v>
+      </c>
+      <c r="B10" s="34">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="34" customFormat="1">
       <c r="A11" s="44" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="34" customFormat="1">
       <c r="A12" s="44" t="s">
-        <v>128</v>
-      </c>
-      <c r="F12" s="34">
+        <v>125</v>
+      </c>
+      <c r="B12" s="34">
         <v>0.5</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="34" customFormat="1">
       <c r="A13" s="44" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="34" customFormat="1">
       <c r="A14" s="44" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="34" customFormat="1">
@@ -70475,30 +70462,30 @@
     </row>
     <row r="16" spans="1:11" s="34" customFormat="1">
       <c r="A16" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="F16" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="34" t="s">
         <v>73</v>
       </c>
       <c r="I16" s="34" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="34" customFormat="1">
+    <row r="17" spans="1:2" s="34" customFormat="1">
       <c r="A17" s="44" t="s">
-        <v>132</v>
-      </c>
-      <c r="F17" s="34">
+        <v>129</v>
+      </c>
+      <c r="B17" s="34">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="34" customFormat="1">
+    <row r="18" spans="1:2" s="34" customFormat="1">
       <c r="A18" s="44"/>
     </row>
-    <row r="19" spans="1:6" s="34" customFormat="1">
+    <row r="19" spans="1:2" s="34" customFormat="1">
       <c r="A19" s="44"/>
     </row>
-    <row r="20" spans="1:6" s="34" customFormat="1">
+    <row r="20" spans="1:2" s="34" customFormat="1">
       <c r="A20" s="44"/>
     </row>
   </sheetData>

</xml_diff>